<commit_message>
I have added the comments for the changes required in the script
</commit_message>
<xml_diff>
--- a/tests/artifact/script/EditProductDetails.xlsx
+++ b/tests/artifact/script/EditProductDetails.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="984">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="986">
   <si>
     <t>target</t>
   </si>
@@ -2454,6 +2454,9 @@
     <t>10000</t>
   </si>
   <si>
+    <t>If the test case is for navigation to business page then we don't want click on add button</t>
+  </si>
+  <si>
     <t>click on add button in Contact page</t>
   </si>
   <si>
@@ -2485,6 +2488,9 @@
   </si>
   <si>
     <t>Milk_Product[NUMBER(${num})=&gt;randomDigits(3)]</t>
+  </si>
+  <si>
+    <t>The test case is for add business Items but the steps are not completed till line 17 it does not add the business item either you name the activity different or finish adding the product before a new activity is started</t>
   </si>
   <si>
     <t>Then user can enter the Product name</t>
@@ -3041,12 +3047,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="37">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3119,6 +3125,13 @@
       <b/>
       <sz val="11"/>
       <color theme="0" tint="-0.0499893185216834"/>
+      <name val="Tahoma"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Tahoma"/>
       <charset val="134"/>
     </font>
@@ -3651,26 +3664,23 @@
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3679,119 +3689,122 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3982,39 +3995,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -7424,34 +7445,34 @@
       <c r="N13" s="52"/>
       <c r="O13" s="44"/>
     </row>
-    <row r="14" s="57" customFormat="1" ht="41" customHeight="1" spans="1:15">
-      <c r="A14" s="58" t="s">
+    <row r="14" s="59" customFormat="1" ht="41" customHeight="1" spans="1:15">
+      <c r="A14" s="60" t="s">
         <v>766</v>
       </c>
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="61" t="s">
         <v>767</v>
       </c>
-      <c r="C14" s="60" t="s">
+      <c r="C14" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="61" t="s">
+      <c r="D14" s="63" t="s">
         <v>447</v>
       </c>
-      <c r="E14" s="61" t="s">
+      <c r="E14" s="63" t="s">
         <v>768</v>
       </c>
-      <c r="F14" s="62" t="s">
+      <c r="F14" s="64" t="s">
         <v>769</v>
       </c>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="66"/>
-      <c r="N14" s="65"/>
-      <c r="O14" s="64"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="66"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="67"/>
+      <c r="O14" s="66"/>
     </row>
     <row r="15" ht="23" customHeight="1" spans="1:15">
       <c r="A15" s="37"/>
@@ -10110,8 +10131,8 @@
   <sheetPr/>
   <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="15.5"/>
@@ -10421,10 +10442,12 @@
       <c r="I12" s="28"/>
       <c r="J12" s="42"/>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="37"/>
+    <row r="13" ht="70" spans="1:10">
+      <c r="A13" s="57" t="s">
+        <v>790</v>
+      </c>
       <c r="B13" s="21" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C13" s="38" t="s">
         <v>30</v>
@@ -10433,10 +10456,10 @@
         <v>576</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
@@ -10445,10 +10468,10 @@
     </row>
     <row r="14" ht="42" spans="1:10">
       <c r="A14" s="20" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>30</v>
@@ -10457,7 +10480,7 @@
         <v>253</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="F14" s="27"/>
       <c r="G14" s="27"/>
@@ -10468,7 +10491,7 @@
     <row r="15" spans="1:10">
       <c r="A15" s="20"/>
       <c r="B15" s="30" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="C15" s="31" t="s">
         <v>30</v>
@@ -10477,7 +10500,7 @@
         <v>253</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="F15" s="33"/>
       <c r="G15" s="27"/>
@@ -10488,7 +10511,7 @@
     <row r="16" spans="1:10">
       <c r="A16" s="20"/>
       <c r="B16" s="30" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="C16" s="31" t="s">
         <v>5</v>
@@ -10497,20 +10520,22 @@
         <v>471</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="G16" s="27"/>
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
       <c r="J16" s="34"/>
     </row>
-    <row r="17" ht="28" spans="1:10">
-      <c r="A17" s="20"/>
+    <row r="17" ht="168" spans="1:10">
+      <c r="A17" s="58" t="s">
+        <v>802</v>
+      </c>
       <c r="B17" s="30" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="C17" s="31" t="s">
         <v>30</v>
@@ -10519,10 +10544,10 @@
         <v>706</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="F17" s="33" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="G17" s="27"/>
       <c r="H17" s="27"/>
@@ -10531,10 +10556,10 @@
     </row>
     <row r="18" ht="28" spans="1:10">
       <c r="A18" s="20" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>30</v>
@@ -10543,7 +10568,7 @@
         <v>253</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="F18" s="27"/>
       <c r="G18" s="27"/>
@@ -10554,7 +10579,7 @@
     <row r="19" ht="28" spans="1:10">
       <c r="A19" s="20"/>
       <c r="B19" s="21" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>30</v>
@@ -10563,7 +10588,7 @@
         <v>253</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="F19" s="27"/>
       <c r="G19" s="27"/>
@@ -10574,7 +10599,7 @@
     <row r="20" ht="28" spans="1:10">
       <c r="A20" s="20"/>
       <c r="B20" s="21" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>30</v>
@@ -10583,10 +10608,10 @@
         <v>707</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="G20" s="27"/>
       <c r="H20" s="27"/>
@@ -10596,7 +10621,7 @@
     <row r="21" spans="1:10">
       <c r="A21" s="20"/>
       <c r="B21" s="21" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>8</v>
@@ -10605,10 +10630,10 @@
         <v>656</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="G21" s="27"/>
       <c r="H21" s="27"/>
@@ -10618,7 +10643,7 @@
     <row r="22" ht="28" spans="1:10">
       <c r="A22" s="20"/>
       <c r="B22" s="21" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>30</v>
@@ -10627,7 +10652,7 @@
         <v>253</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="F22" s="27"/>
       <c r="G22" s="27"/>
@@ -10638,7 +10663,7 @@
     <row r="23" ht="28" spans="1:10">
       <c r="A23" s="20"/>
       <c r="B23" s="21" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>30</v>
@@ -10647,7 +10672,7 @@
         <v>253</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="27"/>
@@ -10658,7 +10683,7 @@
     <row r="24" ht="28" spans="1:10">
       <c r="A24" s="20"/>
       <c r="B24" s="21" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>30</v>
@@ -10667,7 +10692,7 @@
         <v>253</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="27"/>
@@ -10678,7 +10703,7 @@
     <row r="25" ht="28" spans="1:10">
       <c r="A25" s="20"/>
       <c r="B25" s="21" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>30</v>
@@ -10687,10 +10712,10 @@
         <v>707</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="F25" s="32" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
@@ -10700,7 +10725,7 @@
     <row r="26" ht="28" spans="1:10">
       <c r="A26" s="20"/>
       <c r="B26" s="21" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>30</v>
@@ -10709,10 +10734,10 @@
         <v>707</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="F26" s="32" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
@@ -10722,7 +10747,7 @@
     <row r="27" spans="1:10">
       <c r="A27" s="20"/>
       <c r="B27" s="21" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>30</v>
@@ -10731,10 +10756,10 @@
         <v>707</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
@@ -10744,7 +10769,7 @@
     <row r="28" ht="28" spans="1:10">
       <c r="A28" s="20"/>
       <c r="B28" s="21" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="C28" s="26" t="s">
         <v>30</v>
@@ -10753,7 +10778,7 @@
         <v>253</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="F28" s="32"/>
       <c r="G28" s="27"/>
@@ -10763,10 +10788,10 @@
     </row>
     <row r="29" ht="28" spans="1:10">
       <c r="A29" s="20" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="C29" s="26" t="s">
         <v>30</v>
@@ -10775,7 +10800,7 @@
         <v>253</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="F29" s="32"/>
       <c r="G29" s="27"/>
@@ -10786,7 +10811,7 @@
     <row r="30" ht="28" spans="1:10">
       <c r="A30" s="37"/>
       <c r="B30" s="39" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="C30" s="38" t="s">
         <v>30</v>
@@ -10795,7 +10820,7 @@
         <v>253</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="F30" s="28"/>
       <c r="G30" s="28"/>
@@ -10806,7 +10831,7 @@
     <row r="31" ht="28" spans="1:10">
       <c r="A31" s="37"/>
       <c r="B31" s="39" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="C31" s="38" t="s">
         <v>30</v>
@@ -10815,10 +10840,10 @@
         <v>707</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="F31" s="28" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="G31" s="28"/>
       <c r="H31" s="28"/>
@@ -10828,7 +10853,7 @@
     <row r="32" spans="1:10">
       <c r="A32" s="37"/>
       <c r="B32" s="39" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="C32" s="38" t="s">
         <v>30</v>
@@ -10837,7 +10862,7 @@
         <v>253</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="F32" s="28"/>
       <c r="G32" s="28"/>
@@ -10848,7 +10873,7 @@
     <row r="33" ht="28" spans="1:10">
       <c r="A33" s="37"/>
       <c r="B33" s="39" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="C33" s="38" t="s">
         <v>30</v>
@@ -10857,10 +10882,10 @@
         <v>707</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="F33" s="28" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
@@ -10870,7 +10895,7 @@
     <row r="34" ht="28" spans="1:10">
       <c r="A34" s="37"/>
       <c r="B34" s="39" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="C34" s="38" t="s">
         <v>30</v>
@@ -10879,7 +10904,7 @@
         <v>253</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="F34" s="28"/>
       <c r="G34" s="28"/>
@@ -10889,10 +10914,10 @@
     </row>
     <row r="35" ht="28" spans="1:10">
       <c r="A35" s="37" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="C35" s="38" t="s">
         <v>30</v>
@@ -10901,7 +10926,7 @@
         <v>253</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="F35" s="28"/>
       <c r="G35" s="28"/>
@@ -10912,7 +10937,7 @@
     <row r="36" ht="28" spans="1:10">
       <c r="A36" s="37"/>
       <c r="B36" s="39" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="C36" s="38" t="s">
         <v>30</v>
@@ -10921,7 +10946,7 @@
         <v>253</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="F36" s="28"/>
       <c r="G36" s="28"/>
@@ -10932,7 +10957,7 @@
     <row r="37" spans="1:10">
       <c r="A37" s="37"/>
       <c r="B37" s="39" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="C37" s="38" t="s">
         <v>30</v>
@@ -10941,7 +10966,7 @@
         <v>253</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="F37" s="28"/>
       <c r="G37" s="28"/>
@@ -10952,7 +10977,7 @@
     <row r="38" ht="28" spans="1:10">
       <c r="A38" s="37"/>
       <c r="B38" s="39" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="C38" s="38" t="s">
         <v>30</v>
@@ -10961,7 +10986,7 @@
         <v>253</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="F38" s="28"/>
       <c r="G38" s="28"/>
@@ -10971,10 +10996,10 @@
     </row>
     <row r="39" ht="28" spans="1:10">
       <c r="A39" s="37" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="C39" s="26" t="s">
         <v>30</v>
@@ -10983,7 +11008,7 @@
         <v>253</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="F39" s="27"/>
       <c r="G39" s="28"/>
@@ -10994,7 +11019,7 @@
     <row r="40" spans="1:10">
       <c r="A40" s="37"/>
       <c r="B40" s="21" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="C40" s="26" t="s">
         <v>30</v>
@@ -11003,7 +11028,7 @@
         <v>253</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="F40" s="27"/>
       <c r="G40" s="28"/>
@@ -11014,7 +11039,7 @@
     <row r="41" spans="1:10">
       <c r="A41" s="37"/>
       <c r="B41" s="21" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="C41" s="26" t="s">
         <v>30</v>
@@ -11023,7 +11048,7 @@
         <v>576</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="F41" s="28" t="s">
         <v>754</v>
@@ -11036,7 +11061,7 @@
     <row r="42" spans="1:10">
       <c r="A42" s="37"/>
       <c r="B42" s="39" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="C42" s="38" t="s">
         <v>30</v>
@@ -11045,7 +11070,7 @@
         <v>363</v>
       </c>
       <c r="E42" s="28" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="F42" s="28"/>
       <c r="G42" s="28"/>
@@ -11055,7 +11080,7 @@
     </row>
     <row r="43" spans="2:5">
       <c r="B43" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="C43" s="38" t="s">
         <v>30</v>
@@ -11064,7 +11089,7 @@
         <v>253</v>
       </c>
       <c r="E43" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
     </row>
   </sheetData>
@@ -11136,7 +11161,7 @@
   <sheetPr/>
   <dimension ref="A1:O105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="B52" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="A66" workbookViewId="0">
       <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
@@ -11192,7 +11217,7 @@
     </row>
     <row r="2" s="2" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="16" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -11273,10 +11298,10 @@
     </row>
     <row r="5" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A5" s="20" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>30</v>
@@ -11299,7 +11324,7 @@
     <row r="6" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A6" s="20"/>
       <c r="B6" s="21" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="C6" s="26" t="s">
         <v>30</v>
@@ -11308,7 +11333,7 @@
         <v>363</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="F6" s="27"/>
       <c r="G6" s="28"/>
@@ -11331,7 +11356,7 @@
         <v>714</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="F7" s="29"/>
       <c r="G7" s="28"/>
@@ -11347,7 +11372,7 @@
     <row r="8" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A8" s="20"/>
       <c r="B8" s="30" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="C8" s="31" t="s">
         <v>30</v>
@@ -11356,7 +11381,7 @@
         <v>363</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="F8" s="33"/>
       <c r="G8" s="28"/>
@@ -11379,7 +11404,7 @@
         <v>714</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="F9" s="33"/>
       <c r="G9" s="28"/>
@@ -11395,7 +11420,7 @@
     <row r="10" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A10" s="20"/>
       <c r="B10" s="30" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>30</v>
@@ -11404,7 +11429,7 @@
         <v>363</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="F10" s="33"/>
       <c r="G10" s="28"/>
@@ -11419,10 +11444,10 @@
     </row>
     <row r="11" s="4" customFormat="1" ht="22" customHeight="1" spans="1:8">
       <c r="A11" s="20" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>5</v>
@@ -11431,22 +11456,22 @@
         <v>486</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="F11" s="35" t="s">
         <v>774</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" ht="25" customHeight="1" spans="1:15">
       <c r="A12" s="20"/>
       <c r="B12" s="21" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>30</v>
@@ -11455,7 +11480,7 @@
         <v>363</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="28"/>
@@ -11471,7 +11496,7 @@
     <row r="13" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A13" s="37"/>
       <c r="B13" s="21" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="C13" s="38" t="s">
         <v>30</v>
@@ -11480,7 +11505,7 @@
         <v>716</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
@@ -11496,7 +11521,7 @@
     <row r="14" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A14" s="37"/>
       <c r="B14" s="21" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="C14" s="38" t="s">
         <v>30</v>
@@ -11505,7 +11530,7 @@
         <v>714</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
@@ -11520,10 +11545,10 @@
     </row>
     <row r="15" s="4" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A15" s="37" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="C15" s="38" t="s">
         <v>30</v>
@@ -11532,7 +11557,7 @@
         <v>363</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
@@ -11548,7 +11573,7 @@
     <row r="16" s="4" customFormat="1" ht="28" spans="1:15">
       <c r="A16" s="37"/>
       <c r="B16" s="39" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="C16" s="38" t="s">
         <v>30</v>
@@ -11557,13 +11582,13 @@
         <v>650</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="H16" s="28"/>
       <c r="I16" s="28"/>
@@ -11584,7 +11609,7 @@
         <v>714</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
@@ -11600,7 +11625,7 @@
     <row r="18" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A18" s="20"/>
       <c r="B18" s="39" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>5</v>
@@ -11609,10 +11634,10 @@
         <v>49</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="G18" s="28"/>
       <c r="H18" s="27"/>
@@ -11627,7 +11652,7 @@
     <row r="19" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A19" s="20"/>
       <c r="B19" s="21" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>30</v>
@@ -11636,10 +11661,10 @@
         <v>706</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="27"/>
@@ -11677,7 +11702,7 @@
     <row r="21" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A21" s="20"/>
       <c r="B21" s="21" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>30</v>
@@ -11686,10 +11711,10 @@
         <v>692</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="G21" s="28"/>
       <c r="H21" s="27"/>
@@ -11704,7 +11729,7 @@
     <row r="22" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A22" s="37"/>
       <c r="B22" s="39" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="C22" s="38" t="s">
         <v>30</v>
@@ -11713,7 +11738,7 @@
         <v>576</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="F22" s="28" t="s">
         <v>780</v>
@@ -11731,7 +11756,7 @@
     <row r="23" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A23" s="37"/>
       <c r="B23" s="39" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="C23" s="38" t="s">
         <v>30</v>
@@ -11740,7 +11765,7 @@
         <v>576</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="F23" s="28" t="s">
         <v>780</v>
@@ -11758,7 +11783,7 @@
     <row r="24" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A24" s="37"/>
       <c r="B24" s="39" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="C24" s="38" t="s">
         <v>30</v>
@@ -11767,7 +11792,7 @@
         <v>253</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
@@ -11783,7 +11808,7 @@
     <row r="25" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A25" s="37"/>
       <c r="B25" s="21" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="C25" s="38" t="s">
         <v>30</v>
@@ -11792,7 +11817,7 @@
         <v>714</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
@@ -11807,10 +11832,10 @@
     </row>
     <row r="26" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
       <c r="A26" s="37" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="C26" s="38" t="s">
         <v>30</v>
@@ -11819,13 +11844,13 @@
         <v>650</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
@@ -11839,7 +11864,7 @@
     <row r="27" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
       <c r="A27" s="37"/>
       <c r="B27" s="39" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>5</v>
@@ -11848,10 +11873,10 @@
         <v>49</v>
       </c>
       <c r="E27" s="27" t="s">
+        <v>899</v>
+      </c>
+      <c r="F27" s="27" t="s">
         <v>897</v>
-      </c>
-      <c r="F27" s="27" t="s">
-        <v>895</v>
       </c>
       <c r="G27" s="28"/>
       <c r="H27" s="28"/>
@@ -11866,7 +11891,7 @@
     <row r="28" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
       <c r="A28" s="37"/>
       <c r="B28" s="39" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="C28" s="38" t="s">
         <v>30</v>
@@ -11875,13 +11900,13 @@
         <v>650</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="F28" s="27" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="G28" s="28" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="H28" s="28"/>
       <c r="I28" s="28"/>
@@ -11895,7 +11920,7 @@
     <row r="29" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
       <c r="A29" s="37"/>
       <c r="B29" s="39" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="C29" s="26" t="s">
         <v>5</v>
@@ -11904,10 +11929,10 @@
         <v>49</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="F29" s="40" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="G29" s="28"/>
       <c r="H29" s="28"/>
@@ -11922,7 +11947,7 @@
     <row r="30" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
       <c r="A30" s="37"/>
       <c r="B30" s="39" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>30</v>
@@ -11931,7 +11956,7 @@
         <v>363</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="F30" s="27"/>
       <c r="G30" s="28"/>
@@ -11947,7 +11972,7 @@
     <row r="31" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A31" s="20"/>
       <c r="B31" s="21" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="C31" s="26" t="s">
         <v>5</v>
@@ -11972,7 +11997,7 @@
     <row r="32" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A32" s="37"/>
       <c r="B32" s="21" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="C32" s="38" t="s">
         <v>30</v>
@@ -11981,7 +12006,7 @@
         <v>714</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="F32" s="28"/>
       <c r="G32" s="28"/>
@@ -11996,10 +12021,10 @@
     </row>
     <row r="33" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A33" s="37" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="C33" s="38" t="s">
         <v>30</v>
@@ -12008,7 +12033,7 @@
         <v>363</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="F33" s="28"/>
       <c r="G33" s="28"/>
@@ -12024,7 +12049,7 @@
     <row r="34" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A34" s="37"/>
       <c r="B34" s="39" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="C34" s="38" t="s">
         <v>30</v>
@@ -12033,10 +12058,10 @@
         <v>706</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
@@ -12051,7 +12076,7 @@
     <row r="35" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A35" s="37"/>
       <c r="B35" s="39" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="C35" s="38" t="s">
         <v>30</v>
@@ -12060,7 +12085,7 @@
         <v>714</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="G35" s="28"/>
       <c r="H35" s="28"/>
@@ -12075,7 +12100,7 @@
     <row r="36" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A36" s="37"/>
       <c r="B36" s="39" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="C36" s="38" t="s">
         <v>30</v>
@@ -12084,10 +12109,10 @@
         <v>706</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
@@ -12102,7 +12127,7 @@
     <row r="37" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A37" s="37"/>
       <c r="B37" s="39" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="C37" s="38" t="s">
         <v>30</v>
@@ -12111,7 +12136,7 @@
         <v>714</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="G37" s="28"/>
       <c r="H37" s="28"/>
@@ -12126,7 +12151,7 @@
     <row r="38" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A38" s="37"/>
       <c r="B38" s="39" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="C38" s="38" t="s">
         <v>30</v>
@@ -12135,10 +12160,10 @@
         <v>706</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="G38" s="28"/>
       <c r="H38" s="28"/>
@@ -12153,7 +12178,7 @@
     <row r="39" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A39" s="37"/>
       <c r="B39" s="39" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="C39" s="38" t="s">
         <v>30</v>
@@ -12162,7 +12187,7 @@
         <v>714</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
@@ -12177,7 +12202,7 @@
     <row r="40" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A40" s="37"/>
       <c r="B40" s="39" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="C40" s="38" t="s">
         <v>30</v>
@@ -12186,7 +12211,7 @@
         <v>576</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="F40" s="27" t="s">
         <v>780</v>
@@ -12204,7 +12229,7 @@
     <row r="41" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A41" s="37"/>
       <c r="B41" s="39" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="C41" s="38" t="s">
         <v>30</v>
@@ -12213,7 +12238,7 @@
         <v>576</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="F41" s="27" t="s">
         <v>780</v>
@@ -12231,7 +12256,7 @@
     <row r="42" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A42" s="37"/>
       <c r="B42" s="39" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="C42" s="38" t="s">
         <v>30</v>
@@ -12240,7 +12265,7 @@
         <v>253</v>
       </c>
       <c r="E42" s="28" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="F42" s="27"/>
       <c r="G42" s="28"/>
@@ -12256,7 +12281,7 @@
     <row r="43" s="1" customFormat="1" spans="1:15">
       <c r="A43" s="37"/>
       <c r="B43" s="39" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="C43" s="26" t="s">
         <v>30</v>
@@ -12265,7 +12290,7 @@
         <v>363</v>
       </c>
       <c r="E43" s="28" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="F43" s="27"/>
       <c r="G43" s="28"/>
@@ -12281,7 +12306,7 @@
     <row r="44" s="1" customFormat="1" spans="1:15">
       <c r="A44" s="37"/>
       <c r="B44" s="39" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="C44" s="38" t="s">
         <v>30</v>
@@ -12290,10 +12315,10 @@
         <v>366</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="F44" s="28" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="G44" s="28"/>
       <c r="H44" s="28"/>
@@ -12308,7 +12333,7 @@
     <row r="45" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A45" s="37"/>
       <c r="B45" s="21" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="C45" s="38" t="s">
         <v>30</v>
@@ -12317,7 +12342,7 @@
         <v>714</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="F45" s="28"/>
       <c r="G45" s="28"/>
@@ -12332,10 +12357,10 @@
     </row>
     <row r="46" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A46" s="37" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="B46" s="39" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="C46" s="38" t="s">
         <v>30</v>
@@ -12344,7 +12369,7 @@
         <v>363</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
@@ -12360,7 +12385,7 @@
     <row r="47" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A47" s="37"/>
       <c r="B47" s="39" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="C47" s="38" t="s">
         <v>30</v>
@@ -12369,10 +12394,10 @@
         <v>706</v>
       </c>
       <c r="E47" s="28" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="G47" s="28"/>
       <c r="H47" s="28"/>
@@ -12387,7 +12412,7 @@
     <row r="48" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A48" s="37"/>
       <c r="B48" s="39" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="C48" s="38" t="s">
         <v>30</v>
@@ -12396,10 +12421,10 @@
         <v>692</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="G48" s="28"/>
       <c r="H48" s="28"/>
@@ -12414,7 +12439,7 @@
     <row r="49" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A49" s="37"/>
       <c r="B49" s="39" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="C49" s="38" t="s">
         <v>30</v>
@@ -12423,10 +12448,10 @@
         <v>706</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="G49" s="28"/>
       <c r="H49" s="28"/>
@@ -12441,7 +12466,7 @@
     <row r="50" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A50" s="37"/>
       <c r="B50" s="39" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="C50" s="38" t="s">
         <v>30</v>
@@ -12450,10 +12475,10 @@
         <v>706</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="G50" s="28"/>
       <c r="H50" s="28"/>
@@ -12468,7 +12493,7 @@
     <row r="51" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A51" s="37"/>
       <c r="B51" s="39" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="C51" s="38" t="s">
         <v>30</v>
@@ -12477,7 +12502,7 @@
         <v>363</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="G51" s="28"/>
       <c r="H51" s="28"/>
@@ -12492,7 +12517,7 @@
     <row r="52" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A52" s="37"/>
       <c r="B52" s="39" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="C52" s="38" t="s">
         <v>30</v>
@@ -12501,10 +12526,10 @@
         <v>706</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="G52" s="28"/>
       <c r="H52" s="28"/>
@@ -12519,7 +12544,7 @@
     <row r="53" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A53" s="37"/>
       <c r="B53" s="39" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="C53" s="38" t="s">
         <v>30</v>
@@ -12528,7 +12553,7 @@
         <v>363</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="F53" s="28"/>
       <c r="G53" s="28"/>
@@ -12544,7 +12569,7 @@
     <row r="54" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A54" s="37"/>
       <c r="B54" s="39" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="C54" s="38" t="s">
         <v>30</v>
@@ -12553,10 +12578,10 @@
         <v>692</v>
       </c>
       <c r="E54" s="28" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="F54" s="42" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="G54" s="28"/>
       <c r="H54" s="28"/>
@@ -12571,7 +12596,7 @@
     <row r="55" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A55" s="37"/>
       <c r="B55" s="39" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="C55" s="38" t="s">
         <v>30</v>
@@ -12580,7 +12605,7 @@
         <v>576</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="F55" s="36">
         <v>15000</v>
@@ -12598,7 +12623,7 @@
     <row r="56" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A56" s="37"/>
       <c r="B56" s="39" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="C56" s="38" t="s">
         <v>30</v>
@@ -12607,7 +12632,7 @@
         <v>576</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="F56" s="28" t="s">
         <v>780</v>
@@ -12625,7 +12650,7 @@
     <row r="57" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A57" s="37"/>
       <c r="B57" s="39" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="C57" s="38" t="s">
         <v>30</v>
@@ -12634,7 +12659,7 @@
         <v>576</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="F57" s="28" t="s">
         <v>780</v>
@@ -12652,7 +12677,7 @@
     <row r="58" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A58" s="37"/>
       <c r="B58" s="39" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="C58" s="38" t="s">
         <v>30</v>
@@ -12661,7 +12686,7 @@
         <v>576</v>
       </c>
       <c r="E58" s="28" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="F58" s="28" t="s">
         <v>780</v>
@@ -12679,7 +12704,7 @@
     <row r="59" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A59" s="37"/>
       <c r="B59" s="39" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="C59" s="38" t="s">
         <v>30</v>
@@ -12688,10 +12713,10 @@
         <v>692</v>
       </c>
       <c r="E59" s="28" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="F59" s="42" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="G59" s="28"/>
       <c r="H59" s="28"/>
@@ -12706,7 +12731,7 @@
     <row r="60" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A60" s="37"/>
       <c r="B60" s="39" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="C60" s="38" t="s">
         <v>5</v>
@@ -12715,10 +12740,10 @@
         <v>471</v>
       </c>
       <c r="E60" s="28" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="F60" s="28" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="G60" s="28"/>
       <c r="H60" s="28"/>
@@ -12733,7 +12758,7 @@
     <row r="61" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A61" s="37"/>
       <c r="B61" s="39" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="C61" s="38" t="s">
         <v>5</v>
@@ -12742,10 +12767,10 @@
         <v>471</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="F61" s="28" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="G61" s="28"/>
       <c r="H61" s="28"/>
@@ -12760,7 +12785,7 @@
     <row r="62" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A62" s="37"/>
       <c r="B62" s="39" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="C62" s="38" t="s">
         <v>5</v>
@@ -12769,16 +12794,16 @@
         <v>486</v>
       </c>
       <c r="E62" s="28" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="F62" s="28" t="s">
         <v>774</v>
       </c>
       <c r="G62" s="28" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="H62" s="28" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="I62" s="28"/>
       <c r="J62" s="42"/>
@@ -12791,7 +12816,7 @@
     <row r="63" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A63" s="37"/>
       <c r="B63" s="39" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="C63" s="38" t="s">
         <v>5</v>
@@ -12800,13 +12825,13 @@
         <v>506</v>
       </c>
       <c r="E63" s="28" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="F63" s="28" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="G63" s="28" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="H63" s="28"/>
       <c r="I63" s="28"/>
@@ -12820,7 +12845,7 @@
     <row r="64" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A64" s="37"/>
       <c r="B64" s="39" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="C64" s="38" t="s">
         <v>5</v>
@@ -12829,10 +12854,10 @@
         <v>471</v>
       </c>
       <c r="E64" s="28" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="F64" s="28" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="G64" s="28"/>
       <c r="H64" s="28"/>
@@ -12847,7 +12872,7 @@
     <row r="65" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A65" s="37"/>
       <c r="B65" s="39" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="C65" s="38" t="s">
         <v>30</v>
@@ -12856,7 +12881,7 @@
         <v>576</v>
       </c>
       <c r="E65" s="28" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="F65" s="28" t="s">
         <v>780</v>
@@ -12874,7 +12899,7 @@
     <row r="66" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A66" s="37"/>
       <c r="B66" s="39" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="C66" s="38" t="s">
         <v>30</v>
@@ -12883,10 +12908,10 @@
         <v>706</v>
       </c>
       <c r="E66" s="28" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="F66" s="28" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="G66" s="28"/>
       <c r="H66" s="28"/>
@@ -12901,7 +12926,7 @@
     <row r="67" s="1" customFormat="1" spans="1:15">
       <c r="A67" s="37"/>
       <c r="B67" s="39" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="C67" s="38" t="s">
         <v>30</v>
@@ -12910,7 +12935,7 @@
         <v>576</v>
       </c>
       <c r="E67" s="28" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="F67" s="27" t="s">
         <v>780</v>
@@ -12928,7 +12953,7 @@
     <row r="68" s="1" customFormat="1" spans="1:15">
       <c r="A68" s="37"/>
       <c r="B68" s="39" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="C68" s="38" t="s">
         <v>30</v>
@@ -12937,7 +12962,7 @@
         <v>576</v>
       </c>
       <c r="E68" s="28" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="F68" s="27" t="s">
         <v>780</v>
@@ -12955,7 +12980,7 @@
     <row r="69" s="1" customFormat="1" spans="1:15">
       <c r="A69" s="37"/>
       <c r="B69" s="39" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="C69" s="38" t="s">
         <v>30</v>
@@ -12964,7 +12989,7 @@
         <v>253</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="F69" s="27"/>
       <c r="G69" s="28"/>
@@ -12980,7 +13005,7 @@
     <row r="70" s="1" customFormat="1" spans="1:15">
       <c r="A70" s="37"/>
       <c r="B70" s="39" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="C70" s="26" t="s">
         <v>30</v>
@@ -12989,7 +13014,7 @@
         <v>363</v>
       </c>
       <c r="E70" s="28" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="F70" s="27"/>
       <c r="G70" s="28"/>
@@ -13005,7 +13030,7 @@
     <row r="71" s="1" customFormat="1" spans="1:15">
       <c r="A71" s="37"/>
       <c r="B71" s="39" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="C71" s="38" t="s">
         <v>30</v>
@@ -13014,7 +13039,7 @@
         <v>366</v>
       </c>
       <c r="E71" s="28" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="F71" s="36">
         <v>1000</v>
@@ -13032,7 +13057,7 @@
     <row r="72" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A72" s="37"/>
       <c r="B72" s="21" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="C72" s="38" t="s">
         <v>30</v>
@@ -13041,7 +13066,7 @@
         <v>714</v>
       </c>
       <c r="E72" s="28" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="F72" s="28"/>
       <c r="G72" s="28"/>
@@ -13056,10 +13081,10 @@
     </row>
     <row r="73" s="1" customFormat="1" ht="28" spans="1:15">
       <c r="A73" s="37" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="B73" s="39" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="C73" s="38" t="s">
         <v>30</v>
@@ -13068,10 +13093,10 @@
         <v>576</v>
       </c>
       <c r="E73" s="28" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="F73" s="28" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="G73" s="28"/>
       <c r="H73" s="28"/>
@@ -13086,7 +13111,7 @@
     <row r="74" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A74" s="37"/>
       <c r="B74" s="39" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="C74" s="38" t="s">
         <v>30</v>
@@ -13095,10 +13120,10 @@
         <v>692</v>
       </c>
       <c r="E74" s="28" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="F74" s="28" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="G74" s="28"/>
       <c r="H74" s="28"/>
@@ -13113,7 +13138,7 @@
     <row r="75" s="1" customFormat="1" spans="1:15">
       <c r="A75" s="37"/>
       <c r="B75" s="39" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="C75" s="38" t="s">
         <v>30</v>
@@ -13122,7 +13147,7 @@
         <v>576</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="F75" s="27" t="s">
         <v>780</v>
@@ -13140,7 +13165,7 @@
     <row r="76" s="1" customFormat="1" spans="1:15">
       <c r="A76" s="37"/>
       <c r="B76" s="39" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="C76" s="38" t="s">
         <v>30</v>
@@ -13149,7 +13174,7 @@
         <v>576</v>
       </c>
       <c r="E76" s="28" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="F76" s="27" t="s">
         <v>780</v>
@@ -13167,7 +13192,7 @@
     <row r="77" s="1" customFormat="1" spans="1:15">
       <c r="A77" s="37"/>
       <c r="B77" s="39" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="C77" s="38" t="s">
         <v>30</v>
@@ -13176,7 +13201,7 @@
         <v>253</v>
       </c>
       <c r="E77" s="28" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="F77" s="27"/>
       <c r="G77" s="28"/>
@@ -13192,7 +13217,7 @@
     <row r="78" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A78" s="37"/>
       <c r="B78" s="39" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="C78" s="38" t="s">
         <v>30</v>
@@ -13201,7 +13226,7 @@
         <v>363</v>
       </c>
       <c r="E78" s="28" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="F78" s="27"/>
       <c r="G78" s="28"/>

</xml_diff>